<commit_message>
Mapeamento placa GR-CPCI-TEST 029 - JP21, JP22, JP23 e JP24 terminado
</commit_message>
<xml_diff>
--- a/Como/Manuais/GR-PCI-XC5V/GR-CPCI-TESTE_029_pinagem/GR-CPCI-TESTE_029_pinagem.xlsx
+++ b/Como/Manuais/GR-PCI-XC5V/GR-CPCI-TESTE_029_pinagem/GR-CPCI-TESTE_029_pinagem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="21075" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="JP21 - JP22" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="117">
   <si>
     <t>JP21</t>
   </si>
@@ -327,6 +327,69 @@
   </si>
   <si>
     <t>GENIO91</t>
+  </si>
+  <si>
+    <t>J27</t>
+  </si>
+  <si>
+    <t>M28</t>
+  </si>
+  <si>
+    <t>GENIO82</t>
+  </si>
+  <si>
+    <t>L28</t>
+  </si>
+  <si>
+    <t>GENIO84</t>
+  </si>
+  <si>
+    <t>N27</t>
+  </si>
+  <si>
+    <t>GENIO86</t>
+  </si>
+  <si>
+    <t>K27</t>
+  </si>
+  <si>
+    <t>GENIO88</t>
+  </si>
+  <si>
+    <t>GENIO83</t>
+  </si>
+  <si>
+    <t>G28</t>
+  </si>
+  <si>
+    <t>GENIO85</t>
+  </si>
+  <si>
+    <t>L26</t>
+  </si>
+  <si>
+    <t>GENIO87</t>
+  </si>
+  <si>
+    <t>AF31</t>
+  </si>
+  <si>
+    <t>GENIO89</t>
+  </si>
+  <si>
+    <t>N28</t>
+  </si>
+  <si>
+    <t>GENIO80</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>GENIO81</t>
+  </si>
+  <si>
+    <t>NC</t>
   </si>
 </sst>
 </file>
@@ -793,126 +856,120 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -931,6 +988,24 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -940,31 +1015,19 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1270,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,313 +1350,313 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="46"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="24" t="s">
+      <c r="F4" s="61"/>
+      <c r="G4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="K4" s="50" t="s">
+      <c r="H4" s="58"/>
+      <c r="I4" s="59"/>
+      <c r="K4" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="56"/>
     </row>
     <row r="5" spans="2:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="41"/>
+      <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="18" t="s">
         <v>2</v>
       </c>
       <c r="J5" s="2"/>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="55"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="50"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="12">
         <v>4</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>1</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="15">
         <v>2</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>5</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="12" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="55"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="50"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="14">
         <v>3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <v>4</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>6</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="14" t="s">
         <v>21</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="55"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="14">
         <v>2</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <v>6</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>7</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="1"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="58"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="53"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="27">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>7</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <v>8</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="13">
         <v>8</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="14" t="s">
         <v>25</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="14">
         <v>57</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>9</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <v>10</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="13">
         <v>56</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="16" t="s">
+      <c r="I10" s="14" t="s">
         <v>27</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="14">
         <v>58</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>11</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <v>12</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="13">
         <v>55</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="14" t="s">
         <v>29</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="14">
         <v>59</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>13</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <v>14</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="13">
         <v>54</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="14" t="s">
         <v>31</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="30">
         <v>60</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>15</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <v>16</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="19">
         <v>53</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J13" s="3"/>
@@ -1601,272 +1664,272 @@
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27" t="s">
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="24" t="s">
+      <c r="F17" s="61"/>
+      <c r="G17" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="10" t="s">
+      <c r="F18" s="41"/>
+      <c r="G18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>12</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="15">
         <v>2</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="10">
         <v>13</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="27">
         <v>11</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="16">
         <v>4</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="13">
         <v>14</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="H20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="27">
         <v>10</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>5</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <v>6</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="13">
         <v>15</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="H21" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="16">
+      <c r="D22" s="14">
         <v>9</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>7</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <v>8</v>
       </c>
-      <c r="G22" s="15">
+      <c r="G22" s="13">
         <v>16</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="14" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="16">
+      <c r="D23" s="14">
         <v>49</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>9</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <v>10</v>
       </c>
-      <c r="G23" s="15">
+      <c r="G23" s="13">
         <v>48</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="14" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="27">
         <v>50</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>11</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="16">
         <v>12</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="13">
         <v>47</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="H24" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I24" s="16" t="s">
+      <c r="I24" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="27">
         <v>51</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>13</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <v>14</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="13">
         <v>46</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="H25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="I25" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="21">
         <v>52</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="6">
         <v>15</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="17">
         <v>16</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="19">
         <v>45</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="21" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1894,8 +1957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,481 +1974,582 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="46"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="47"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27" t="s">
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="24" t="s">
+      <c r="F4" s="61"/>
+      <c r="G4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26"/>
-      <c r="K4" s="50" t="s">
+      <c r="H4" s="58"/>
+      <c r="I4" s="59"/>
+      <c r="K4" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
-      <c r="O4" s="52"/>
+      <c r="L4" s="55"/>
+      <c r="M4" s="55"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="56"/>
     </row>
     <row r="5" spans="2:15" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="41"/>
+      <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="20" t="s">
+      <c r="I5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="54"/>
-      <c r="M5" s="54"/>
-      <c r="N5" s="54"/>
-      <c r="O5" s="55"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="50"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="39">
         <v>20</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>1</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="15">
         <v>2</v>
       </c>
-      <c r="G6" s="59">
+      <c r="G6" s="37">
         <v>21</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="53"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="55"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="50"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="24">
         <v>19</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <v>4</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="22">
         <v>22</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="53"/>
-      <c r="L7" s="54"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="55"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="24">
         <v>18</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <v>6</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="22">
         <v>23</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="31" t="s">
+      <c r="I8" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
-      <c r="M8" s="57"/>
-      <c r="N8" s="57"/>
-      <c r="O8" s="58"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="53"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="24">
         <v>17</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>7</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <v>8</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="22">
         <v>24</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="24" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="34">
+      <c r="D10" s="27">
         <v>41</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>9</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <v>10</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="25">
         <v>40</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="H10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="27" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="24">
         <v>42</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>11</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <v>12</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="22">
         <v>39</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="24" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="24">
         <v>43</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>13</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <v>14</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="22">
         <v>38</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H12" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="24" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="36">
         <v>44</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="6">
         <v>15</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <v>16</v>
       </c>
-      <c r="G13" s="41">
+      <c r="G13" s="34">
         <v>37</v>
       </c>
-      <c r="H13" s="42" t="s">
+      <c r="H13" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="36" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="46"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="2:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27" t="s">
+      <c r="C17" s="58"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="24" t="s">
+      <c r="F17" s="61"/>
+      <c r="G17" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="26"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
     </row>
     <row r="18" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="10" t="s">
+      <c r="F18" s="41"/>
+      <c r="G18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="6">
+      <c r="B19" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="33">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4">
         <v>1</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="15">
         <v>2</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
+      <c r="G19" s="31">
+        <v>29</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="33" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="7">
+      <c r="B20" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="24">
+        <v>27</v>
+      </c>
+      <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="16">
         <v>4</v>
       </c>
-      <c r="G20" s="29"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
+      <c r="G20" s="25">
+        <v>30</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="27" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="7">
+      <c r="B21" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="24">
+        <v>26</v>
+      </c>
+      <c r="E21" s="5">
         <v>5</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="16">
         <v>6</v>
       </c>
-      <c r="G21" s="29"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31"/>
+      <c r="G21" s="22">
+        <v>32</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="7">
+      <c r="B22" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="24">
+        <v>25</v>
+      </c>
+      <c r="E22" s="5">
         <v>7</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <v>8</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
+      <c r="G22" s="25">
+        <v>31</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="7">
+      <c r="B23" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="24">
+        <v>33</v>
+      </c>
+      <c r="E23" s="5">
         <v>9</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="16">
         <v>10</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+      <c r="G23" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="7">
+      <c r="B24" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="24">
+        <v>34</v>
+      </c>
+      <c r="E24" s="5">
         <v>11</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="16">
         <v>12</v>
       </c>
-      <c r="G24" s="29"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+      <c r="G24" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="7">
+      <c r="B25" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="24">
+        <v>35</v>
+      </c>
+      <c r="E25" s="5">
         <v>13</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="16">
         <v>14</v>
       </c>
-      <c r="G25" s="29"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
+      <c r="G25" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="24" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="26" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="8">
+      <c r="B26" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="36">
+        <v>36</v>
+      </c>
+      <c r="E26" s="6">
         <v>15</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="17">
         <v>16</v>
       </c>
-      <c r="G26" s="41"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
+      <c r="G26" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="K4:O4"/>
     <mergeCell ref="K5:O8"/>
     <mergeCell ref="E18:F18"/>
@@ -2393,13 +2557,9 @@
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="B2:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>